<commit_message>
Second Me did not work out
</commit_message>
<xml_diff>
--- a/CH-131 Table Transformation.xlsx
+++ b/CH-131 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C204C12-87AE-4205-AF52-638C93147AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763D150B-C1E9-4966-A5FE-FB6E80A5B565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="EDA" sheetId="1" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Me1" sheetId="4" r:id="rId4"/>
-    <sheet name="Me2)" sheetId="5" r:id="rId5"/>
+    <sheet name="Me2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2932,21 +2932,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F23862-5661-42CF-8908-CC4547756974}">
-  <dimension ref="B1:P25"/>
+  <dimension ref="B1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.8984375" customWidth="1"/>
-    <col min="3" max="3" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="10.296875" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.19921875" style="1" customWidth="1"/>
     <col min="12" max="13" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.09765625" style="1" bestFit="1" customWidth="1"/>
@@ -3253,145 +3248,105 @@
         <v>12</v>
       </c>
     </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="str" cm="1">
+        <f t="array" ref="C13:H17">C3:C7&amp;D2:I2</f>
+        <v>AQuantity</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <v>APayment</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <v>ADiscount</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <v>AQuantity</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <v>APayment</v>
+      </c>
+      <c r="H13" s="1" t="str">
+        <v>ADiscount</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="str">
+        <v>BQuantity</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <v>BPayment</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <v>BDiscount</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <v>BQuantity</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <v>BPayment</v>
+      </c>
+      <c r="H14" s="1" t="str">
+        <v>BDiscount</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="str">
+        <v>CQuantity</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <v>CPayment</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <v>CDiscount</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <v>CQuantity</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <v>CPayment</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <v>CDiscount</v>
+      </c>
+    </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="str" cm="1">
-        <f t="array" ref="D16:G25">_xlfn.HSTACK(_xlfn.VSTACK(C3:C7,C3:C7),_xlfn.WRAPROWS(_xlfn.TOCOL(D3:I7),3))</f>
-        <v>A</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1">
-        <v>100</v>
-      </c>
-      <c r="G16" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="str">
+        <v>DQuantity</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <v>DPayment</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <v>DDiscount</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <v>DQuantity</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <v>DPayment</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <v>DDiscount</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="str">
+        <v>EQuantity</v>
+      </c>
       <c r="D17" s="1" t="str">
-        <v>B</v>
-      </c>
-      <c r="E17" s="1">
-        <v>3</v>
-      </c>
-      <c r="F17" s="1">
-        <v>50</v>
-      </c>
-      <c r="G17" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="str">
-        <v>C</v>
-      </c>
-      <c r="E18" s="1">
-        <v>2</v>
-      </c>
-      <c r="F18" s="1">
-        <v>50</v>
-      </c>
-      <c r="G18" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="1" t="str">
-        <v>D</v>
-      </c>
-      <c r="E19" s="1">
-        <v>3</v>
-      </c>
-      <c r="F19" s="1">
-        <v>120</v>
-      </c>
-      <c r="G19" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="str">
-        <v>E</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3</v>
-      </c>
-      <c r="F20" s="1">
-        <v>75</v>
-      </c>
-      <c r="G20" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="str">
-        <v>A</v>
-      </c>
-      <c r="E21" s="1">
-        <v>3</v>
-      </c>
-      <c r="F21" s="1">
-        <v>140</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="1" t="str">
-        <v>B</v>
-      </c>
-      <c r="E22" s="1">
-        <v>4</v>
-      </c>
-      <c r="F22" s="1">
-        <v>80</v>
-      </c>
-      <c r="G22" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="1" t="str">
-        <v>C</v>
-      </c>
-      <c r="E23" s="1">
-        <v>3</v>
-      </c>
-      <c r="F23" s="1">
-        <v>80</v>
-      </c>
-      <c r="G23" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="1" t="str">
-        <v>D</v>
-      </c>
-      <c r="E24" s="1">
-        <v>5</v>
-      </c>
-      <c r="F24" s="1">
-        <v>90</v>
-      </c>
-      <c r="G24" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="1" t="str">
-        <v>E</v>
-      </c>
-      <c r="E25" s="1">
-        <v>3</v>
-      </c>
-      <c r="F25" s="1">
-        <v>90</v>
-      </c>
-      <c r="G25" s="1">
-        <v>12</v>
+        <v>EPayment</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <v>EDiscount</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <v>EQuantity</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <v>EPayment</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <v>EDiscount</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second me, poor, but works
</commit_message>
<xml_diff>
--- a/CH-131 Table Transformation.xlsx
+++ b/CH-131 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763D150B-C1E9-4966-A5FE-FB6E80A5B565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D556AF01-1E40-4815-BE68-9C40A7D19634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2932,10 +2932,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F23862-5661-42CF-8908-CC4547756974}">
-  <dimension ref="B1:P17"/>
+  <dimension ref="B1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3248,105 +3248,204 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="str" cm="1">
-        <f t="array" ref="C13:H17">C3:C7&amp;D2:I2</f>
-        <v>AQuantity</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <v>APayment</v>
-      </c>
-      <c r="E13" s="1" t="str">
-        <v>ADiscount</v>
-      </c>
-      <c r="F13" s="1" t="str">
-        <v>AQuantity</v>
-      </c>
-      <c r="G13" s="1" t="str">
-        <v>APayment</v>
-      </c>
-      <c r="H13" s="1" t="str">
-        <v>ADiscount</v>
-      </c>
-    </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="str">
-        <v>BQuantity</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <v>BPayment</v>
-      </c>
-      <c r="E14" s="1" t="str">
-        <v>BDiscount</v>
-      </c>
-      <c r="F14" s="1" t="str">
-        <v>BQuantity</v>
+      <c r="C14" s="1" t="str" cm="1">
+        <f t="array" aca="1" ref="C14:C18" ca="1">_xlfn.BYROW(C3:I7,_xlfn.LAMBDA(_xlpm.r,_xlfn.TEXTJOIN(",",,OFFSET(_xlpm.r,0,0,1,4))&amp;"|"&amp;OFFSET(_xlpm.r,0,0,1,1)&amp;","&amp;_xlfn.TEXTJOIN(",",,OFFSET(_xlpm.r,0,4,1,3))))</f>
+        <v>A,1,100,10|A,3,50,4</v>
+      </c>
+      <c r="F14" s="1" t="str" cm="1">
+        <f t="array" aca="1" ref="F14:I23" ca="1">_xlfn.DROP(_xlfn._xlws.SORT(_xlfn.HSTACK(_xlfn.DROP(_xlfn.REDUCE("",C14:C18,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,",","|")))),1),MOD(_xlfn.SEQUENCE(10,1,0),2)),5),,-1)</f>
+        <v>A</v>
       </c>
       <c r="G14" s="1" t="str">
-        <v>BPayment</v>
+        <f ca="1"/>
+        <v>1</v>
       </c>
       <c r="H14" s="1" t="str">
-        <v>BDiscount</v>
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f ca="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="str">
-        <v>CQuantity</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <v>CPayment</v>
-      </c>
-      <c r="E15" s="1" t="str">
-        <v>CDiscount</v>
+        <f ca="1"/>
+        <v>B,2,50,5|B,3,120,17</v>
       </c>
       <c r="F15" s="1" t="str">
-        <v>CQuantity</v>
+        <f ca="1"/>
+        <v>B</v>
       </c>
       <c r="G15" s="1" t="str">
-        <v>CPayment</v>
+        <f ca="1"/>
+        <v>2</v>
       </c>
       <c r="H15" s="1" t="str">
-        <v>CDiscount</v>
+        <f ca="1"/>
+        <v>50</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f ca="1"/>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="str">
-        <v>DQuantity</v>
-      </c>
-      <c r="D16" s="1" t="str">
-        <v>DPayment</v>
-      </c>
-      <c r="E16" s="1" t="str">
-        <v>DDiscount</v>
+        <f ca="1"/>
+        <v>C,3,75,4|C,3,140,20</v>
       </c>
       <c r="F16" s="1" t="str">
-        <v>DQuantity</v>
+        <f ca="1"/>
+        <v>C</v>
       </c>
       <c r="G16" s="1" t="str">
-        <v>DPayment</v>
+        <f ca="1"/>
+        <v>3</v>
       </c>
       <c r="H16" s="1" t="str">
-        <v>DDiscount</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+        <f ca="1"/>
+        <v>75</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="str">
-        <v>EQuantity</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <v>EPayment</v>
-      </c>
-      <c r="E17" s="1" t="str">
-        <v>EDiscount</v>
+        <f ca="1"/>
+        <v>D,4,80,6|D,3,80,8</v>
       </c>
       <c r="F17" s="1" t="str">
-        <v>EQuantity</v>
+        <f ca="1"/>
+        <v>D</v>
       </c>
       <c r="G17" s="1" t="str">
-        <v>EPayment</v>
+        <f ca="1"/>
+        <v>4</v>
       </c>
       <c r="H17" s="1" t="str">
-        <v>EDiscount</v>
+        <f ca="1"/>
+        <v>80</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f ca="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="str">
+        <f ca="1"/>
+        <v>E,5,90,7|E,3,90,12</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f ca="1"/>
+        <v>E</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f ca="1"/>
+        <v>5</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f ca="1"/>
+        <v>90</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f ca="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="str">
+        <f ca="1"/>
+        <v>A</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f ca="1"/>
+        <v>50</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f ca="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="str">
+        <f ca="1"/>
+        <v>B</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f ca="1"/>
+        <v>120</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f ca="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="str">
+        <f ca="1"/>
+        <v>C</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <f ca="1"/>
+        <v>140</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f ca="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="1" t="str">
+        <f ca="1"/>
+        <v>D</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="H22" s="1" t="str">
+        <f ca="1"/>
+        <v>80</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f ca="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="1" t="str">
+        <f ca="1"/>
+        <v>E</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f ca="1"/>
+        <v>3</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f ca="1"/>
+        <v>90</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f ca="1"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>